<commit_message>
Before remove SFC manual command return
</commit_message>
<xml_diff>
--- a/archive/HMIAlarms.xlsx
+++ b/archive/HMIAlarms.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DiscreteAlarms" sheetId="1" r:id="R4a4e0efbde46423d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DiscreteAlarms" sheetId="1" r:id="R3578fc0020784813"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -9793,7 +9793,7 @@
     <x:t>logonManualAction</x:t>
   </x:si>
   <x:si>
-    <x:t>SERIALID &lt;field ref="0" /&gt; : USERID &lt;field ref="1" /&gt; : Manual Action : &lt;field ref="2" /&gt; &lt;field ref="3" /&gt; &lt;field ref="4" /&gt; &lt;field ref="5" /&gt;</x:t>
+    <x:t>SERIALID &lt;field ref="0" /&gt; : USERID &lt;field ref="1" /&gt; : Manual Action : &lt;field ref="2" /&gt; &lt;field ref="3" /&gt; &lt;field ref="4" /&gt; : oldValue  &lt;field ref="6" /&gt; : newValue &lt;field ref="7" /&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;ref id = 0; type = AlarmTag; Tag = interfaceVerify.numSerial; DisplayType = Decimal; Length = 6;&gt;
@@ -9801,7 +9801,8 @@
 &lt;ref id = 2; type = AlarmTag; Tag = interfaceVerify.pendingClass; DisplayType = Text; Length = 10;&gt;
 &lt;ref id = 3; type = AlarmTag; Tag = interfaceVerify.pendingInstance; DisplayType = Text; Length = 20;&gt;
 &lt;ref id = 4; type = AlarmTag; Tag = interfaceVerify.pendingTarget; DisplayType = Text; Length = 10;&gt;
-&lt;ref id = 5; type = AlarmTag; Tag = interfaceVerify.pendingCommand; DisplayType = Text; Length = 5;&gt;
+&lt;ref id = 6; type = AlarmTag; Tag = interfaceVerify.valueOld; DisplayType = Text; Length = 10;&gt;
+&lt;ref id = 7; type = AlarmTag; Tag = interfaceVerify.valueNew; DisplayType = Text; Length = 10;&gt;
 </x:t>
   </x:si>
   <x:si>

</xml_diff>